<commit_message>
Fixed lab link form
</commit_message>
<xml_diff>
--- a/xlsform/link.xlsx
+++ b/xlsform/link.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>type</t>
   </si>
@@ -24,6 +24,9 @@
     <t>label</t>
   </si>
   <si>
+    <t>help</t>
+  </si>
+  <si>
     <t>required</t>
   </si>
   <si>
@@ -87,7 +90,10 @@
     <t>srepeat</t>
   </si>
   <si>
-    <t>New Result</t>
+    <t>New Link</t>
+  </si>
+  <si>
+    <t>Scan the matching pair of barcodes in sequence -- ST barcode then Lab barcode</t>
   </si>
   <si>
     <t>barcode</t>
@@ -99,61 +105,46 @@
     <t>ST Barcode</t>
   </si>
   <si>
-    <t>select_one stype</t>
-  </si>
-  <si>
     <t>labid</t>
   </si>
   <si>
     <t>Lab Barcode</t>
   </si>
   <si>
-    <t>quick search('stypes')</t>
-  </si>
-  <si>
-    <t>select_one condition</t>
+    <t>end repeat</t>
+  </si>
+  <si>
+    <t>geopoint</t>
+  </si>
+  <si>
+    <t>store_gps</t>
+  </si>
+  <si>
+    <t>GPS Coordinates</t>
+  </si>
+  <si>
+    <t>list name</t>
+  </si>
+  <si>
+    <t>region_key</t>
+  </si>
+  <si>
+    <t>facility_key</t>
+  </si>
+  <si>
+    <t>rider</t>
+  </si>
+  <si>
+    <t>rider_key</t>
+  </si>
+  <si>
+    <t>stype</t>
+  </si>
+  <si>
+    <t>stype_key</t>
   </si>
   <si>
     <t>condition</t>
-  </si>
-  <si>
-    <t>Specimen Condition</t>
-  </si>
-  <si>
-    <t>quick search('conditions')</t>
-  </si>
-  <si>
-    <t>end repeat</t>
-  </si>
-  <si>
-    <t>geopoint</t>
-  </si>
-  <si>
-    <t>store_gps</t>
-  </si>
-  <si>
-    <t>GPS Coordinates</t>
-  </si>
-  <si>
-    <t>list name</t>
-  </si>
-  <si>
-    <t>region_key</t>
-  </si>
-  <si>
-    <t>facility_key</t>
-  </si>
-  <si>
-    <t>rider</t>
-  </si>
-  <si>
-    <t>rider_key</t>
-  </si>
-  <si>
-    <t>stype</t>
-  </si>
-  <si>
-    <t>stype_key</t>
   </si>
   <si>
     <t>cond_key</t>
@@ -224,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -232,6 +223,9 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -289,8 +283,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="25.57"/>
-    <col customWidth="1" min="5" max="5" width="45.0"/>
-    <col customWidth="1" min="6" max="6" width="14.71"/>
+    <col customWidth="1" min="6" max="6" width="45.0"/>
+    <col customWidth="1" min="7" max="7" width="14.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -306,175 +300,168 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="8"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8"/>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="9"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="C9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="7"/>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="6"/>
+      <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="C11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="6" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>12</v>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -490,98 +477,98 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="C4" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="C5" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="11"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -596,19 +583,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>